<commit_message>
UI Revamp now has subsections
</commit_message>
<xml_diff>
--- a/Project Requirements/Forge Gantt Chart.xlsx
+++ b/Project Requirements/Forge Gantt Chart.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Plan</t>
   </si>
@@ -174,12 +174,33 @@
   <si>
     <t>WEEK</t>
   </si>
+  <si>
+    <t xml:space="preserve">    CAD file upload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Model Interactivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    QR Vrok.it Connection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    A360/Fusion360 File Access</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    File Conversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Hardware Detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Viewable VR Model</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -267,8 +288,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +351,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,7 +429,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -439,6 +489,21 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="8" borderId="0" xfId="6" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -908,13 +973,13 @@
   <dimension ref="B2:BQ34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="26.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.375" style="2" customWidth="1"/>
     <col min="3" max="5" width="7.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.375" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.25" style="7" customWidth="1"/>
@@ -1254,13 +1319,13 @@
     </row>
     <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C10" s="16">
         <v>11</v>
       </c>
       <c r="D10" s="16">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="E10" s="16">
         <v>0</v>
@@ -1273,202 +1338,468 @@
       </c>
     </row>
     <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="21">
+        <v>12</v>
+      </c>
+      <c r="D11" s="21">
+        <v>5</v>
+      </c>
+      <c r="E11" s="21">
+        <v>0</v>
+      </c>
+      <c r="F11" s="21">
+        <v>0</v>
+      </c>
+      <c r="G11" s="22">
+        <v>0</v>
+      </c>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="23"/>
+      <c r="Y11" s="23"/>
+      <c r="Z11" s="23"/>
+      <c r="AA11" s="23"/>
+      <c r="AB11" s="23"/>
+      <c r="AC11" s="24"/>
+      <c r="AD11" s="24"/>
+      <c r="AE11" s="24"/>
+      <c r="AF11" s="24"/>
+      <c r="AG11" s="24"/>
+      <c r="AH11" s="24"/>
+      <c r="AI11" s="24"/>
+      <c r="AJ11" s="24"/>
+      <c r="AK11" s="24"/>
+      <c r="AL11" s="24"/>
+      <c r="AM11" s="24"/>
+      <c r="AN11" s="24"/>
+      <c r="AO11" s="24"/>
+      <c r="AP11" s="24"/>
+      <c r="AQ11" s="24"/>
+      <c r="AR11" s="24"/>
+    </row>
+    <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="21">
+        <v>12</v>
+      </c>
+      <c r="D12" s="21">
+        <v>5</v>
+      </c>
+      <c r="E12" s="21">
+        <v>0</v>
+      </c>
+      <c r="F12" s="21">
+        <v>0</v>
+      </c>
+      <c r="G12" s="22">
+        <v>0</v>
+      </c>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="23"/>
+      <c r="Z12" s="23"/>
+      <c r="AA12" s="23"/>
+      <c r="AB12" s="23"/>
+      <c r="AC12" s="24"/>
+      <c r="AD12" s="24"/>
+      <c r="AE12" s="24"/>
+      <c r="AF12" s="24"/>
+      <c r="AG12" s="24"/>
+      <c r="AH12" s="24"/>
+      <c r="AI12" s="24"/>
+      <c r="AJ12" s="24"/>
+      <c r="AK12" s="24"/>
+      <c r="AL12" s="24"/>
+      <c r="AM12" s="24"/>
+      <c r="AN12" s="24"/>
+      <c r="AO12" s="24"/>
+      <c r="AP12" s="24"/>
+      <c r="AQ12" s="24"/>
+      <c r="AR12" s="24"/>
+    </row>
+    <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="21">
+        <v>12</v>
+      </c>
+      <c r="D13" s="21">
+        <v>5</v>
+      </c>
+      <c r="E13" s="21">
+        <v>0</v>
+      </c>
+      <c r="F13" s="21">
+        <v>0</v>
+      </c>
+      <c r="G13" s="22">
+        <v>0</v>
+      </c>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23"/>
+      <c r="X13" s="23"/>
+      <c r="Y13" s="23"/>
+      <c r="Z13" s="23"/>
+      <c r="AA13" s="23"/>
+      <c r="AB13" s="23"/>
+      <c r="AC13" s="24"/>
+      <c r="AD13" s="24"/>
+      <c r="AE13" s="24"/>
+      <c r="AF13" s="24"/>
+      <c r="AG13" s="24"/>
+      <c r="AH13" s="24"/>
+      <c r="AI13" s="24"/>
+      <c r="AJ13" s="24"/>
+      <c r="AK13" s="24"/>
+      <c r="AL13" s="24"/>
+      <c r="AM13" s="24"/>
+      <c r="AN13" s="24"/>
+      <c r="AO13" s="24"/>
+      <c r="AP13" s="24"/>
+      <c r="AQ13" s="24"/>
+      <c r="AR13" s="24"/>
+    </row>
+    <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="21">
+        <v>17</v>
+      </c>
+      <c r="D14" s="21">
+        <v>5</v>
+      </c>
+      <c r="E14" s="21">
+        <v>0</v>
+      </c>
+      <c r="F14" s="21">
+        <v>0</v>
+      </c>
+      <c r="G14" s="22">
+        <v>0</v>
+      </c>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23"/>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="23"/>
+      <c r="Z14" s="23"/>
+      <c r="AA14" s="23"/>
+      <c r="AB14" s="23"/>
+      <c r="AC14" s="24"/>
+      <c r="AD14" s="24"/>
+      <c r="AE14" s="24"/>
+      <c r="AF14" s="24"/>
+      <c r="AG14" s="24"/>
+      <c r="AH14" s="24"/>
+      <c r="AI14" s="24"/>
+      <c r="AJ14" s="24"/>
+      <c r="AK14" s="24"/>
+      <c r="AL14" s="24"/>
+      <c r="AM14" s="24"/>
+      <c r="AN14" s="24"/>
+      <c r="AO14" s="24"/>
+      <c r="AP14" s="24"/>
+      <c r="AQ14" s="24"/>
+      <c r="AR14" s="24"/>
+    </row>
+    <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="21">
+        <v>22</v>
+      </c>
+      <c r="D15" s="21">
+        <v>5</v>
+      </c>
+      <c r="E15" s="21">
+        <v>0</v>
+      </c>
+      <c r="F15" s="21">
+        <v>0</v>
+      </c>
+      <c r="G15" s="22">
+        <v>0</v>
+      </c>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="23"/>
+      <c r="Z15" s="23"/>
+      <c r="AA15" s="23"/>
+      <c r="AB15" s="23"/>
+      <c r="AC15" s="24"/>
+      <c r="AD15" s="24"/>
+      <c r="AE15" s="24"/>
+      <c r="AF15" s="24"/>
+      <c r="AG15" s="24"/>
+      <c r="AH15" s="24"/>
+      <c r="AI15" s="24"/>
+      <c r="AJ15" s="24"/>
+      <c r="AK15" s="24"/>
+      <c r="AL15" s="24"/>
+      <c r="AM15" s="24"/>
+      <c r="AN15" s="24"/>
+      <c r="AO15" s="24"/>
+      <c r="AP15" s="24"/>
+      <c r="AQ15" s="24"/>
+      <c r="AR15" s="24"/>
+    </row>
+    <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="21">
+        <v>27</v>
+      </c>
+      <c r="D16" s="21">
+        <v>5</v>
+      </c>
+      <c r="E16" s="21">
+        <v>0</v>
+      </c>
+      <c r="F16" s="21">
+        <v>0</v>
+      </c>
+      <c r="G16" s="22">
+        <v>0</v>
+      </c>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
+      <c r="X16" s="23"/>
+      <c r="Y16" s="23"/>
+      <c r="Z16" s="23"/>
+      <c r="AA16" s="23"/>
+      <c r="AB16" s="23"/>
+      <c r="AC16" s="24"/>
+      <c r="AD16" s="24"/>
+      <c r="AE16" s="24"/>
+      <c r="AF16" s="24"/>
+      <c r="AG16" s="24"/>
+      <c r="AH16" s="24"/>
+      <c r="AI16" s="24"/>
+      <c r="AJ16" s="24"/>
+      <c r="AK16" s="24"/>
+      <c r="AL16" s="24"/>
+      <c r="AM16" s="24"/>
+      <c r="AN16" s="24"/>
+      <c r="AO16" s="24"/>
+      <c r="AP16" s="24"/>
+      <c r="AQ16" s="24"/>
+      <c r="AR16" s="24"/>
+    </row>
+    <row r="17" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="21">
+        <v>32</v>
+      </c>
+      <c r="D17" s="21">
+        <v>5</v>
+      </c>
+      <c r="E17" s="21">
+        <v>0</v>
+      </c>
+      <c r="F17" s="21">
+        <v>0</v>
+      </c>
+      <c r="G17" s="22">
+        <v>0</v>
+      </c>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="23"/>
+      <c r="X17" s="23"/>
+      <c r="Y17" s="23"/>
+      <c r="Z17" s="23"/>
+      <c r="AA17" s="23"/>
+      <c r="AB17" s="23"/>
+      <c r="AC17" s="24"/>
+      <c r="AD17" s="24"/>
+      <c r="AE17" s="24"/>
+      <c r="AF17" s="24"/>
+      <c r="AG17" s="24"/>
+      <c r="AH17" s="24"/>
+      <c r="AI17" s="24"/>
+      <c r="AJ17" s="24"/>
+      <c r="AK17" s="24"/>
+      <c r="AL17" s="24"/>
+      <c r="AM17" s="24"/>
+      <c r="AN17" s="24"/>
+      <c r="AO17" s="24"/>
+      <c r="AP17" s="24"/>
+      <c r="AQ17" s="24"/>
+      <c r="AR17" s="24"/>
+    </row>
+    <row r="18" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="16">
+        <v>11</v>
+      </c>
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
+      <c r="E18" s="16">
+        <v>0</v>
+      </c>
+      <c r="F18" s="16">
+        <v>0</v>
+      </c>
+      <c r="G18" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C19" s="16">
+        <v>11</v>
+      </c>
+      <c r="D19" s="16">
+        <v>1</v>
+      </c>
+      <c r="E19" s="16">
+        <v>0</v>
+      </c>
+      <c r="F19" s="16">
+        <v>0</v>
+      </c>
+      <c r="G19" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="16">
-        <v>4</v>
-      </c>
-      <c r="E11" s="16">
-        <v>0</v>
-      </c>
-      <c r="F11" s="16">
-        <v>0</v>
-      </c>
-      <c r="G11" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="16">
+      <c r="C20" s="16">
+        <v>11</v>
+      </c>
+      <c r="D20" s="16">
+        <v>1</v>
+      </c>
+      <c r="E20" s="16">
+        <v>0</v>
+      </c>
+      <c r="F20" s="16">
+        <v>0</v>
+      </c>
+      <c r="G20" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="16">
+        <v>12</v>
+      </c>
+      <c r="D21" s="16">
+        <v>5</v>
+      </c>
+      <c r="E21" s="16">
+        <v>0</v>
+      </c>
+      <c r="F21" s="16">
+        <v>0</v>
+      </c>
+      <c r="G21" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="16">
+        <v>17</v>
+      </c>
+      <c r="D22" s="16">
+        <v>5</v>
+      </c>
+      <c r="E22" s="16">
+        <v>0</v>
+      </c>
+      <c r="F22" s="16">
+        <v>0</v>
+      </c>
+      <c r="G22" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="16">
+        <v>22</v>
+      </c>
+      <c r="D23" s="16">
+        <v>5</v>
+      </c>
+      <c r="E23" s="16">
+        <v>0</v>
+      </c>
+      <c r="F23" s="16">
+        <v>0</v>
+      </c>
+      <c r="G23" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="16">
-        <v>1</v>
-      </c>
-      <c r="E12" s="16">
-        <v>0</v>
-      </c>
-      <c r="F12" s="16">
-        <v>0</v>
-      </c>
-      <c r="G12" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="16">
-        <v>20</v>
-      </c>
-      <c r="D13" s="16">
-        <v>3</v>
-      </c>
-      <c r="E13" s="16">
-        <v>0</v>
-      </c>
-      <c r="F13" s="16">
-        <v>0</v>
-      </c>
-      <c r="G13" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="16">
-        <v>23</v>
-      </c>
-      <c r="D14" s="16">
-        <v>3</v>
-      </c>
-      <c r="E14" s="16">
-        <v>0</v>
-      </c>
-      <c r="F14" s="16">
-        <v>0</v>
-      </c>
-      <c r="G14" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="16">
-        <v>26</v>
-      </c>
-      <c r="D15" s="16">
-        <v>4</v>
-      </c>
-      <c r="E15" s="16">
-        <v>0</v>
-      </c>
-      <c r="F15" s="16">
-        <v>0</v>
-      </c>
-      <c r="G15" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="16">
-        <v>30</v>
-      </c>
-      <c r="D16" s="16">
-        <v>4</v>
-      </c>
-      <c r="E16" s="16">
-        <v>0</v>
-      </c>
-      <c r="F16" s="16">
-        <v>0</v>
-      </c>
-      <c r="G16" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="16">
-        <v>34</v>
-      </c>
-      <c r="D17" s="16">
-        <v>5</v>
-      </c>
-      <c r="E17" s="16">
-        <v>0</v>
-      </c>
-      <c r="F17" s="16">
-        <v>0</v>
-      </c>
-      <c r="G17" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-    </row>
-    <row r="19" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-    </row>
-    <row r="20" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-    </row>
-    <row r="21" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-    </row>
-    <row r="22" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-    </row>
-    <row r="23" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-    </row>
-    <row r="24" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-    </row>
-    <row r="25" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="16">
+        <v>27</v>
+      </c>
+      <c r="D24" s="16">
+        <v>10</v>
+      </c>
+      <c r="E24" s="16">
+        <v>0</v>
+      </c>
+      <c r="F24" s="16">
+        <v>0</v>
+      </c>
+      <c r="G24" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
@@ -1476,7 +1807,7 @@
       <c r="F25"/>
       <c r="G25"/>
     </row>
-    <row r="26" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
@@ -1484,7 +1815,7 @@
       <c r="F26"/>
       <c r="G26"/>
     </row>
-    <row r="27" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
@@ -1492,7 +1823,7 @@
       <c r="F27"/>
       <c r="G27"/>
     </row>
-    <row r="28" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
@@ -1500,7 +1831,7 @@
       <c r="F28"/>
       <c r="G28"/>
     </row>
-    <row r="29" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
@@ -1508,7 +1839,7 @@
       <c r="F29"/>
       <c r="G29"/>
     </row>
-    <row r="30" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
@@ -1516,7 +1847,7 @@
       <c r="F30"/>
       <c r="G30"/>
     </row>
-    <row r="31" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
@@ -1524,7 +1855,7 @@
       <c r="F31"/>
       <c r="G31"/>
     </row>
-    <row r="32" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>

</xml_diff>

<commit_message>
Made some of the suggested changes to the requirements document
</commit_message>
<xml_diff>
--- a/Project Requirements/Forge Gantt Chart.xlsx
+++ b/Project Requirements/Forge Gantt Chart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Plan</t>
   </si>
@@ -175,32 +175,20 @@
     <t>WEEK</t>
   </si>
   <si>
-    <t xml:space="preserve">    CAD file upload</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Model Interactivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    QR Vrok.it Connection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    A360/Fusion360 File Access</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    File Conversion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Hardware Detection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Viewable VR Model</t>
+    <t>UI Revamp 1</t>
+  </si>
+  <si>
+    <t>UI Revamp 2</t>
+  </si>
+  <si>
+    <t>UI Revamp 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -288,31 +276,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="1" tint="0.24994659260841701"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.24994659260841701"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="7"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,12 +316,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59996337778862885"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,7 +388,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -489,21 +448,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="8" borderId="0" xfId="6" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -516,7 +460,459 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="42">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -682,7 +1078,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="6"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="7"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -970,10 +1366,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:BQ34"/>
+  <dimension ref="B2:BQ30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1012,7 +1408,7 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O3" s="8"/>
       <c r="Q3" s="10"/>
@@ -1316,399 +1712,218 @@
       <c r="G9" s="17">
         <v>0.5</v>
       </c>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C10" s="16">
         <v>11</v>
       </c>
       <c r="D10" s="16">
+        <v>1</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0</v>
+      </c>
+      <c r="F10" s="16">
+        <v>0</v>
+      </c>
+      <c r="G10" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="16">
+        <v>11</v>
+      </c>
+      <c r="D11" s="16">
+        <v>1</v>
+      </c>
+      <c r="E11" s="16">
+        <v>0</v>
+      </c>
+      <c r="F11" s="16">
+        <v>0</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="16">
+        <v>11</v>
+      </c>
+      <c r="D12" s="16">
+        <v>1</v>
+      </c>
+      <c r="E12" s="16">
+        <v>0</v>
+      </c>
+      <c r="F12" s="16">
+        <v>0</v>
+      </c>
+      <c r="G12" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="16">
+        <v>12</v>
+      </c>
+      <c r="D13" s="16">
+        <v>5</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0</v>
+      </c>
+      <c r="F13" s="16">
+        <v>0</v>
+      </c>
+      <c r="G13" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="16">
+        <v>16</v>
+      </c>
+      <c r="D14" s="16">
+        <v>3</v>
+      </c>
+      <c r="E14" s="16">
+        <v>0</v>
+      </c>
+      <c r="F14" s="16">
+        <v>0</v>
+      </c>
+      <c r="G14" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="16">
+        <v>17</v>
+      </c>
+      <c r="D15" s="16">
+        <v>5</v>
+      </c>
+      <c r="E15" s="16">
+        <v>0</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0</v>
+      </c>
+      <c r="G15" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="16">
+        <v>21</v>
+      </c>
+      <c r="D16" s="16">
+        <v>3</v>
+      </c>
+      <c r="E16" s="16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="16">
+        <v>22</v>
+      </c>
+      <c r="D17" s="16">
+        <v>5</v>
+      </c>
+      <c r="E17" s="16">
+        <v>0</v>
+      </c>
+      <c r="F17" s="16">
+        <v>0</v>
+      </c>
+      <c r="G17" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="16">
-        <v>0</v>
-      </c>
-      <c r="F10" s="16">
-        <v>0</v>
-      </c>
-      <c r="G10" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="21">
-        <v>12</v>
-      </c>
-      <c r="D11" s="21">
+      <c r="C18" s="16">
+        <v>26</v>
+      </c>
+      <c r="D18" s="16">
+        <v>3</v>
+      </c>
+      <c r="E18" s="16">
+        <v>0</v>
+      </c>
+      <c r="F18" s="16">
+        <v>0</v>
+      </c>
+      <c r="G18" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="16">
+        <v>27</v>
+      </c>
+      <c r="D19" s="16">
+        <v>10</v>
+      </c>
+      <c r="E19" s="16">
+        <v>0</v>
+      </c>
+      <c r="F19" s="16">
+        <v>0</v>
+      </c>
+      <c r="G19" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="16">
+        <v>33</v>
+      </c>
+      <c r="D20" s="16">
         <v>5</v>
       </c>
-      <c r="E11" s="21">
-        <v>0</v>
-      </c>
-      <c r="F11" s="21">
-        <v>0</v>
-      </c>
-      <c r="G11" s="22">
-        <v>0</v>
-      </c>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="23"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="23"/>
-      <c r="AC11" s="24"/>
-      <c r="AD11" s="24"/>
-      <c r="AE11" s="24"/>
-      <c r="AF11" s="24"/>
-      <c r="AG11" s="24"/>
-      <c r="AH11" s="24"/>
-      <c r="AI11" s="24"/>
-      <c r="AJ11" s="24"/>
-      <c r="AK11" s="24"/>
-      <c r="AL11" s="24"/>
-      <c r="AM11" s="24"/>
-      <c r="AN11" s="24"/>
-      <c r="AO11" s="24"/>
-      <c r="AP11" s="24"/>
-      <c r="AQ11" s="24"/>
-      <c r="AR11" s="24"/>
-    </row>
-    <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="21">
-        <v>12</v>
-      </c>
-      <c r="D12" s="21">
-        <v>5</v>
-      </c>
-      <c r="E12" s="21">
-        <v>0</v>
-      </c>
-      <c r="F12" s="21">
-        <v>0</v>
-      </c>
-      <c r="G12" s="22">
-        <v>0</v>
-      </c>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="23"/>
-      <c r="Z12" s="23"/>
-      <c r="AA12" s="23"/>
-      <c r="AB12" s="23"/>
-      <c r="AC12" s="24"/>
-      <c r="AD12" s="24"/>
-      <c r="AE12" s="24"/>
-      <c r="AF12" s="24"/>
-      <c r="AG12" s="24"/>
-      <c r="AH12" s="24"/>
-      <c r="AI12" s="24"/>
-      <c r="AJ12" s="24"/>
-      <c r="AK12" s="24"/>
-      <c r="AL12" s="24"/>
-      <c r="AM12" s="24"/>
-      <c r="AN12" s="24"/>
-      <c r="AO12" s="24"/>
-      <c r="AP12" s="24"/>
-      <c r="AQ12" s="24"/>
-      <c r="AR12" s="24"/>
-    </row>
-    <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="21">
-        <v>12</v>
-      </c>
-      <c r="D13" s="21">
-        <v>5</v>
-      </c>
-      <c r="E13" s="21">
-        <v>0</v>
-      </c>
-      <c r="F13" s="21">
-        <v>0</v>
-      </c>
-      <c r="G13" s="22">
-        <v>0</v>
-      </c>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="23"/>
-      <c r="X13" s="23"/>
-      <c r="Y13" s="23"/>
-      <c r="Z13" s="23"/>
-      <c r="AA13" s="23"/>
-      <c r="AB13" s="23"/>
-      <c r="AC13" s="24"/>
-      <c r="AD13" s="24"/>
-      <c r="AE13" s="24"/>
-      <c r="AF13" s="24"/>
-      <c r="AG13" s="24"/>
-      <c r="AH13" s="24"/>
-      <c r="AI13" s="24"/>
-      <c r="AJ13" s="24"/>
-      <c r="AK13" s="24"/>
-      <c r="AL13" s="24"/>
-      <c r="AM13" s="24"/>
-      <c r="AN13" s="24"/>
-      <c r="AO13" s="24"/>
-      <c r="AP13" s="24"/>
-      <c r="AQ13" s="24"/>
-      <c r="AR13" s="24"/>
-    </row>
-    <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="21">
-        <v>17</v>
-      </c>
-      <c r="D14" s="21">
-        <v>5</v>
-      </c>
-      <c r="E14" s="21">
-        <v>0</v>
-      </c>
-      <c r="F14" s="21">
-        <v>0</v>
-      </c>
-      <c r="G14" s="22">
-        <v>0</v>
-      </c>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="23"/>
-      <c r="X14" s="23"/>
-      <c r="Y14" s="23"/>
-      <c r="Z14" s="23"/>
-      <c r="AA14" s="23"/>
-      <c r="AB14" s="23"/>
-      <c r="AC14" s="24"/>
-      <c r="AD14" s="24"/>
-      <c r="AE14" s="24"/>
-      <c r="AF14" s="24"/>
-      <c r="AG14" s="24"/>
-      <c r="AH14" s="24"/>
-      <c r="AI14" s="24"/>
-      <c r="AJ14" s="24"/>
-      <c r="AK14" s="24"/>
-      <c r="AL14" s="24"/>
-      <c r="AM14" s="24"/>
-      <c r="AN14" s="24"/>
-      <c r="AO14" s="24"/>
-      <c r="AP14" s="24"/>
-      <c r="AQ14" s="24"/>
-      <c r="AR14" s="24"/>
-    </row>
-    <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="21">
-        <v>22</v>
-      </c>
-      <c r="D15" s="21">
-        <v>5</v>
-      </c>
-      <c r="E15" s="21">
-        <v>0</v>
-      </c>
-      <c r="F15" s="21">
-        <v>0</v>
-      </c>
-      <c r="G15" s="22">
-        <v>0</v>
-      </c>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="23"/>
-      <c r="X15" s="23"/>
-      <c r="Y15" s="23"/>
-      <c r="Z15" s="23"/>
-      <c r="AA15" s="23"/>
-      <c r="AB15" s="23"/>
-      <c r="AC15" s="24"/>
-      <c r="AD15" s="24"/>
-      <c r="AE15" s="24"/>
-      <c r="AF15" s="24"/>
-      <c r="AG15" s="24"/>
-      <c r="AH15" s="24"/>
-      <c r="AI15" s="24"/>
-      <c r="AJ15" s="24"/>
-      <c r="AK15" s="24"/>
-      <c r="AL15" s="24"/>
-      <c r="AM15" s="24"/>
-      <c r="AN15" s="24"/>
-      <c r="AO15" s="24"/>
-      <c r="AP15" s="24"/>
-      <c r="AQ15" s="24"/>
-      <c r="AR15" s="24"/>
-    </row>
-    <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="21">
-        <v>27</v>
-      </c>
-      <c r="D16" s="21">
-        <v>5</v>
-      </c>
-      <c r="E16" s="21">
-        <v>0</v>
-      </c>
-      <c r="F16" s="21">
-        <v>0</v>
-      </c>
-      <c r="G16" s="22">
-        <v>0</v>
-      </c>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="23"/>
-      <c r="Y16" s="23"/>
-      <c r="Z16" s="23"/>
-      <c r="AA16" s="23"/>
-      <c r="AB16" s="23"/>
-      <c r="AC16" s="24"/>
-      <c r="AD16" s="24"/>
-      <c r="AE16" s="24"/>
-      <c r="AF16" s="24"/>
-      <c r="AG16" s="24"/>
-      <c r="AH16" s="24"/>
-      <c r="AI16" s="24"/>
-      <c r="AJ16" s="24"/>
-      <c r="AK16" s="24"/>
-      <c r="AL16" s="24"/>
-      <c r="AM16" s="24"/>
-      <c r="AN16" s="24"/>
-      <c r="AO16" s="24"/>
-      <c r="AP16" s="24"/>
-      <c r="AQ16" s="24"/>
-      <c r="AR16" s="24"/>
-    </row>
-    <row r="17" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="21">
-        <v>32</v>
-      </c>
-      <c r="D17" s="21">
-        <v>5</v>
-      </c>
-      <c r="E17" s="21">
-        <v>0</v>
-      </c>
-      <c r="F17" s="21">
-        <v>0</v>
-      </c>
-      <c r="G17" s="22">
-        <v>0</v>
-      </c>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="23"/>
-      <c r="X17" s="23"/>
-      <c r="Y17" s="23"/>
-      <c r="Z17" s="23"/>
-      <c r="AA17" s="23"/>
-      <c r="AB17" s="23"/>
-      <c r="AC17" s="24"/>
-      <c r="AD17" s="24"/>
-      <c r="AE17" s="24"/>
-      <c r="AF17" s="24"/>
-      <c r="AG17" s="24"/>
-      <c r="AH17" s="24"/>
-      <c r="AI17" s="24"/>
-      <c r="AJ17" s="24"/>
-      <c r="AK17" s="24"/>
-      <c r="AL17" s="24"/>
-      <c r="AM17" s="24"/>
-      <c r="AN17" s="24"/>
-      <c r="AO17" s="24"/>
-      <c r="AP17" s="24"/>
-      <c r="AQ17" s="24"/>
-      <c r="AR17" s="24"/>
-    </row>
-    <row r="18" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="16">
-        <v>11</v>
-      </c>
-      <c r="D18" s="16">
-        <v>1</v>
-      </c>
-      <c r="E18" s="16">
-        <v>0</v>
-      </c>
-      <c r="F18" s="16">
-        <v>0</v>
-      </c>
-      <c r="G18" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="16">
-        <v>11</v>
-      </c>
-      <c r="D19" s="16">
-        <v>1</v>
-      </c>
-      <c r="E19" s="16">
-        <v>0</v>
-      </c>
-      <c r="F19" s="16">
-        <v>0</v>
-      </c>
-      <c r="G19" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="16">
-        <v>11</v>
-      </c>
-      <c r="D20" s="16">
-        <v>1</v>
-      </c>
       <c r="E20" s="16">
         <v>0</v>
       </c>
@@ -1719,87 +1934,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="16">
-        <v>12</v>
-      </c>
-      <c r="D21" s="16">
-        <v>5</v>
-      </c>
-      <c r="E21" s="16">
-        <v>0</v>
-      </c>
-      <c r="F21" s="16">
-        <v>0</v>
-      </c>
-      <c r="G21" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="16">
-        <v>17</v>
-      </c>
-      <c r="D22" s="16">
-        <v>5</v>
-      </c>
-      <c r="E22" s="16">
-        <v>0</v>
-      </c>
-      <c r="F22" s="16">
-        <v>0</v>
-      </c>
-      <c r="G22" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="16">
-        <v>22</v>
-      </c>
-      <c r="D23" s="16">
-        <v>5</v>
-      </c>
-      <c r="E23" s="16">
-        <v>0</v>
-      </c>
-      <c r="F23" s="16">
-        <v>0</v>
-      </c>
-      <c r="G23" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="16">
-        <v>27</v>
-      </c>
-      <c r="D24" s="16">
-        <v>10</v>
-      </c>
-      <c r="E24" s="16">
-        <v>0</v>
-      </c>
-      <c r="F24" s="16">
-        <v>0</v>
-      </c>
-      <c r="G24" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+    </row>
+    <row r="23" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+    </row>
+    <row r="25" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
@@ -1807,7 +1974,7 @@
       <c r="F25"/>
       <c r="G25"/>
     </row>
-    <row r="26" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
@@ -1815,7 +1982,7 @@
       <c r="F26"/>
       <c r="G26"/>
     </row>
-    <row r="27" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
@@ -1823,7 +1990,7 @@
       <c r="F27"/>
       <c r="G27"/>
     </row>
-    <row r="28" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
@@ -1831,7 +1998,7 @@
       <c r="F28"/>
       <c r="G28"/>
     </row>
-    <row r="29" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
@@ -1839,7 +2006,7 @@
       <c r="F29"/>
       <c r="G29"/>
     </row>
-    <row r="30" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
@@ -1847,76 +2014,148 @@
       <c r="F30"/>
       <c r="G30"/>
     </row>
-    <row r="31" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-    </row>
-    <row r="32" spans="2:44" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32"/>
-    </row>
-    <row r="33" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-    </row>
-    <row r="34" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="I9:BP34">
-    <cfRule type="expression" dxfId="9" priority="1">
+  <conditionalFormatting sqref="I15:BP15 I17:BP17 I19:BP19 I21:BP30 I10:BP13 I9 K9:BP9">
+    <cfRule type="expression" dxfId="41" priority="33">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="40" priority="35">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="39" priority="36">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="38" priority="37">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="37" priority="38">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="36" priority="39">
       <formula>I$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="35" priority="43">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="12">
+    <cfRule type="expression" dxfId="34" priority="44">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35:BP35">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="B31:BP31">
+    <cfRule type="expression" dxfId="33" priority="34">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:BP8">
+    <cfRule type="expression" dxfId="32" priority="40">
+      <formula>I$8=period_selected</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:BP14">
+    <cfRule type="expression" dxfId="31" priority="25">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="26">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="27">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="28">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="29">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="30">
+      <formula>I$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="31">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="32">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16:BP16">
+    <cfRule type="expression" dxfId="23" priority="17">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="18">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="19">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="20">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="21">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="22">
+      <formula>I$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="23">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18:BP18">
+    <cfRule type="expression" dxfId="15" priority="9">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="10">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="11">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="12">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>I$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="15">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="16">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20:BP20">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>I$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>I$8=period_selected</formula>
+      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made changes to the gantt chart
</commit_message>
<xml_diff>
--- a/Project Requirements/Forge Gantt Chart.xlsx
+++ b/Project Requirements/Forge Gantt Chart.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Plan</t>
   </si>
@@ -157,16 +157,10 @@
     <t>File Conversion</t>
   </si>
   <si>
-    <t>Hardware Detection</t>
-  </si>
-  <si>
     <t>Viewable VR Model</t>
   </si>
   <si>
     <t>Forge VR Explorer</t>
-  </si>
-  <si>
-    <t>UI Revamp</t>
   </si>
   <si>
     <t>TASKS</t>
@@ -277,7 +271,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +310,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -388,7 +388,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -448,6 +448,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1078,7 +1081,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="7"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="8"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1366,10 +1369,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:BQ30"/>
+  <dimension ref="B2:BQ28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1385,7 +1388,7 @@
   <sheetData>
     <row r="2" spans="2:69" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -1408,7 +1411,7 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O3" s="8"/>
       <c r="Q3" s="10"/>
@@ -1480,7 +1483,7 @@
     </row>
     <row r="7" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>3</v>
@@ -1499,7 +1502,7 @@
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J7" s="4"/>
     </row>
@@ -1710,9 +1713,10 @@
         <v>8</v>
       </c>
       <c r="G9" s="17">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="J9" s="10"/>
+      <c r="O9" s="20"/>
     </row>
     <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
@@ -1796,7 +1800,7 @@
     </row>
     <row r="14" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="16">
         <v>16</v>
@@ -1836,7 +1840,7 @@
     </row>
     <row r="16" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" s="16">
         <v>21</v>
@@ -1859,10 +1863,10 @@
         <v>18</v>
       </c>
       <c r="C17" s="16">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D17" s="16">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E17" s="16">
         <v>0</v>
@@ -1876,13 +1880,13 @@
     </row>
     <row r="18" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" s="16">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D18" s="16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E18" s="16">
         <v>0</v>
@@ -1894,45 +1898,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="16">
-        <v>27</v>
-      </c>
-      <c r="D19" s="16">
-        <v>10</v>
-      </c>
-      <c r="E19" s="16">
-        <v>0</v>
-      </c>
-      <c r="F19" s="16">
-        <v>0</v>
-      </c>
-      <c r="G19" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="16">
-        <v>33</v>
-      </c>
-      <c r="D20" s="16">
-        <v>5</v>
-      </c>
-      <c r="E20" s="16">
-        <v>0</v>
-      </c>
-      <c r="F20" s="16">
-        <v>0</v>
-      </c>
-      <c r="G20" s="17">
-        <v>0</v>
-      </c>
+    <row r="19" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
     </row>
     <row r="21" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21"/>
@@ -1998,27 +1978,11 @@
       <c r="F28"/>
       <c r="G28"/>
     </row>
-    <row r="29" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="G29"/>
-    </row>
-    <row r="30" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="I15:BP15 I17:BP17 I19:BP19 I21:BP30 I10:BP13 I9 K9:BP9">
+  <conditionalFormatting sqref="I15:BP15 I17:BP17 I19:BP28 I10:BP13 I9 K9:BP9">
     <cfRule type="expression" dxfId="41" priority="33">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -2044,7 +2008,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31:BP31">
+  <conditionalFormatting sqref="B29:BP29">
     <cfRule type="expression" dxfId="33" priority="34">
       <formula>TRUE</formula>
     </cfRule>
@@ -2107,32 +2071,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:BP18">
-    <cfRule type="expression" dxfId="15" priority="9">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="10">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="11">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="12">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="13">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14">
-      <formula>I$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="15">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="16">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20:BP20">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>